<commit_message>
Se adjunta el desarrollo de seguridad a la celda robotica
</commit_message>
<xml_diff>
--- a/01 Documentación/04 Taller celdas robotizadas/Análisis de riesgos celda Robótica Soldadura.xlsx
+++ b/01 Documentación/04 Taller celdas robotizadas/Análisis de riesgos celda Robótica Soldadura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leo7s\Documents\Universidad\03 APM\04 Gitrespository\Proyecto_APM\01 Documentación\04 Taller celdas robotizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFCFF32-2492-4D85-8296-4EE0D974C58F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AD6C76-0C69-4EE8-B6EE-44D6E00A53F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1610,8 +1610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Se desarrolla el informe ejecutivo del taller
</commit_message>
<xml_diff>
--- a/01 Documentación/04 Taller celdas robotizadas/Análisis de riesgos celda Robótica Soldadura.xlsx
+++ b/01 Documentación/04 Taller celdas robotizadas/Análisis de riesgos celda Robótica Soldadura.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leo7s\Documents\Universidad\03 APM\04 Gitrespository\Proyecto_APM\01 Documentación\04 Taller celdas robotizadas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j2seb\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AD6C76-0C69-4EE8-B6EE-44D6E00A53F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F92712-600F-44EA-BAAD-FEC28E15E844}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,15 +57,9 @@
     <t>Cerradura con candado para no permitir cerrar la puerta.</t>
   </si>
   <si>
-    <t>Ingreso de personal en la Celda Robótica</t>
-  </si>
-  <si>
     <t>Clasificación</t>
   </si>
   <si>
-    <t>Funcionamiento anormal de la celda</t>
-  </si>
-  <si>
     <t>Gravedad G2, Frecuencia F1, Posibilidad P1</t>
   </si>
   <si>
@@ -78,9 +72,6 @@
     <t>Parada de emergencia</t>
   </si>
   <si>
-    <t>Golpe del Robot a los operarios</t>
-  </si>
-  <si>
     <t>Gravedad G2, Frecuencia F1 , Posibilidad P1</t>
   </si>
   <si>
@@ -111,9 +102,6 @@
     <t>Control de Proceso</t>
   </si>
   <si>
-    <t>Fuga de gases usados en el proceso de soldadura</t>
-  </si>
-  <si>
     <t>PL a</t>
   </si>
   <si>
@@ -138,9 +126,6 @@
     <t>Switch Principal de energia electrica de  la celda que se puede bloquear en posición de apagado</t>
   </si>
   <si>
-    <t>Mala Posición Ergonomica de los operarios al cargar los perfiles, descargar el marco de bicicleta y ubicar los perfiles en la matriz</t>
-  </si>
-  <si>
     <t>Gravedad G1, Frecuencia F2  , Posibilidad P1</t>
   </si>
   <si>
@@ -159,9 +144,6 @@
     <t>Señalización de prohibición de acceso</t>
   </si>
   <si>
-    <t>El robot se mueve en la celda cuando se realizan operaciones de mantenimento e inspección. Posibilidad que el robot se golpee y cause lesiones al operario.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Asegurar que el robot esté detenido  cuando la puerta este abierta. </t>
   </si>
   <si>
@@ -177,25 +159,13 @@
     <t>Diseño de un carro de Carga donde se puedan ubicar y retirar las partes con una posición ergonómica</t>
   </si>
   <si>
-    <t>Posicionador de piezas inicia el giro cuando el operario está cerca</t>
-  </si>
-  <si>
     <t>Sensores de presencia - Ausencia</t>
   </si>
   <si>
-    <t>Daño a la visión de los operarios  de la fabrica</t>
-  </si>
-  <si>
     <t>Severidad G2, Frecuencia F1, Probabilidad P1</t>
   </si>
   <si>
     <t>Evitar que la contaminación visual salga de la zona de soldadura.</t>
-  </si>
-  <si>
-    <t>Cercamiento en malla</t>
-  </si>
-  <si>
-    <t>Daño por quemaduras debido a la soldadura</t>
   </si>
   <si>
     <t>Evitar la cercania del operario a la operación de soldadura</t>
@@ -211,9 +181,6 @@
 • Alarma industrial</t>
   </si>
   <si>
-    <t>Incendio de la celda</t>
-  </si>
-  <si>
     <t>Evitar materiales inflamables
 al interior de la celda robotizada</t>
   </si>
@@ -223,13 +190,246 @@
   </si>
   <si>
     <t>Funcionamiento de la celda</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rg1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Funcionamiento anormal de la celda</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Rg2: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Golpe del Robot a los operarios</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Rg3: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Daño a la visión de los operarios  de la fabrica</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Rg 4: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Daño por quemaduras debido a la soldadura</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rg5:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Incendio de la celda</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rg6:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Ingreso de personal en la Celda Robótica</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rg7:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Fuga de gases usados en el proceso de soldadura</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rg8:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> El robot se mueve en la celda cuando se realizan operaciones de mantenimento e inspección. Posibilidad que el robot se golpee y cause lesiones al operario.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rg 9:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Mala Posición Ergonomica de los operarios al cargar los perfiles, descargar el marco de bicicleta y ubicar los perfiles en la matriz</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rg 10:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Posicionador de piezas inicia el giro cuando el operario está cerca</t>
+    </r>
+  </si>
+  <si>
+    <t>Cercamiento lámina</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +453,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -337,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -393,6 +601,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,13 +671,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>468313</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>896619</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>1087229</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -504,13 +715,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>309678</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>33132</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1044272</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>1107627</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -548,13 +759,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>116416</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>195860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1388465</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>1006083</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -592,13 +803,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>74083</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>232833</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1427358</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>974725</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -636,13 +847,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>359834</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>201085</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1165225</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>1008381</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -741,13 +952,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>58805</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>62804</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1468904</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2920</xdr:colOff>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>930405</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -802,13 +1013,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>165286</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>70037</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1275901</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>1184462</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -863,7 +1074,7 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>288251</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>131033</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="909132" cy="908372"/>
@@ -919,13 +1130,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>325590</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>104167</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1083780</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>590549</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -980,13 +1191,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>200688</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>33131</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1238793</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>968568</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1023,58 +1234,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>421834</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>40230</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1044272</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1121405</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE39ACC0-DA49-4980-971D-21B468660690}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8497377" y="3436100"/>
-          <a:ext cx="626248" cy="1084985"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
       <xdr:colOff>134426</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>100314</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1392345</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>724397</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1091,7 +1258,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1112,13 +1279,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>283514</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>141907</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1241729</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>1088121</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1135,7 +1302,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1156,13 +1323,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>53505</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>49696</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>895796</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>1121208</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1179,7 +1346,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1200,13 +1367,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>728870</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>291796</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1378175</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>973125</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1223,7 +1390,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1243,15 +1410,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>356814</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>69071</xdr:rowOff>
+      <xdr:colOff>382415</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>631536</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1182508</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>783078</xdr:rowOff>
+      <xdr:colOff>1208109</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1345543</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1267,15 +1434,59 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8432357" y="18845745"/>
-          <a:ext cx="825694" cy="706387"/>
+          <a:off x="8789263" y="8193558"/>
+          <a:ext cx="825694" cy="714007"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>210745</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>64593</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1241481</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>999439</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Imagen 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6470A00E-9CA5-4AA6-800C-634AA68B6417}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8592745" y="9589593"/>
+          <a:ext cx="1030736" cy="934846"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1608,27 +1819,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:Q20"/>
+  <dimension ref="B3:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="21.5546875" style="1" customWidth="1"/>
-    <col min="9" max="10" width="9.109375" style="1"/>
-    <col min="12" max="16384" width="9.109375" style="1"/>
+    <col min="4" max="4" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="2" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:17" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
@@ -1636,7 +1847,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="15" t="s">
         <v>2</v>
@@ -1651,317 +1862,336 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>15</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="2:17" ht="156.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:17" ht="156.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="20"/>
       <c r="C5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="13" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>21</v>
       </c>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:17" ht="156.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20"/>
-      <c r="C6" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="19" t="s">
+      <c r="C6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="19" t="s">
-        <v>15</v>
-      </c>
       <c r="F6" s="8" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:17" ht="156.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="C7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="F7" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" ht="156.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="9" t="s">
+      <c r="C8" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="20"/>
+      <c r="C9" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="20"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="20"/>
+      <c r="C13" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="2:17" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14"/>
+      <c r="Q14"/>
+    </row>
+    <row r="15" spans="2:17" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="2:17" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="2:12" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="2:12" ht="98.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="5"/>
+      <c r="H18" s="3"/>
+      <c r="L18"/>
     </row>
-    <row r="9" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H9" s="5"/>
+    <row r="19" spans="2:12" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="17"/>
+      <c r="C19" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="J19"/>
+      <c r="K19" s="1"/>
     </row>
-    <row r="10" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="20"/>
-      <c r="C10" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="7"/>
+    <row r="20" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="18"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="K20" s="1"/>
     </row>
-    <row r="11" spans="2:17" ht="78" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11" s="5"/>
-      <c r="I11"/>
-      <c r="Q11"/>
+    <row r="21" spans="2:12" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="23"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
     </row>
-    <row r="12" spans="2:17" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="3"/>
+    <row r="22" spans="2:12" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="23"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
     </row>
-    <row r="13" spans="2:17" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="2:17" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="2:17" ht="98.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H15" s="3"/>
-      <c r="L15"/>
-    </row>
-    <row r="16" spans="2:17" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="17"/>
-      <c r="C16" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H16" s="7"/>
-      <c r="J16"/>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="2:11" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="17"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17" s="7"/>
-      <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="2:11" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="17"/>
-      <c r="C18" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="2:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="17"/>
-      <c r="C19" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="2:11" s="12" customFormat="1" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="18"/>
-      <c r="C20" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" s="14"/>
-      <c r="K20" s="11"/>
+    <row r="23" spans="2:12" s="12" customFormat="1" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="23"/>
+      <c r="K23" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="B4:B11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="B4:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="B18:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1975,7 +2205,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1987,7 +2217,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se ultiman detalles y se generan los links de entrega
</commit_message>
<xml_diff>
--- a/01 Documentación/04 Taller celdas robotizadas/Análisis de riesgos celda Robótica Soldadura.xlsx
+++ b/01 Documentación/04 Taller celdas robotizadas/Análisis de riesgos celda Robótica Soldadura.xlsx
@@ -5,18 +5,21 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j2seb\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leo7s\Documents\Universidad\03 APM\04 Gitrespository\Proyecto_APM\01 Documentación\04 Taller celdas robotizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F92712-600F-44EA-BAAD-FEC28E15E844}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB38D96B-A1A9-4B78-9C8A-C60B9BC44905}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$21</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
@@ -183,10 +186,6 @@
   <si>
     <t>Evitar materiales inflamables
 al interior de la celda robotizada</t>
-  </si>
-  <si>
-    <t>Señal de "prohibido el ingreso
- de material inflamable"</t>
   </si>
   <si>
     <t>Funcionamiento de la celda</t>
@@ -423,6 +422,10 @@
   </si>
   <si>
     <t>Cercamiento lámina</t>
+  </si>
+  <si>
+    <t>Señal de "prohibido el ingreso, Colocación de un extintor a la entrada de la celda
+ de material inflamable"</t>
   </si>
 </sst>
 </file>
@@ -580,14 +583,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -601,8 +598,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -634,7 +637,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>988464</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>588634</xdr:rowOff>
+      <xdr:rowOff>592444</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -676,9 +679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>896619</xdr:colOff>
+      <xdr:colOff>892809</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>1087229</xdr:rowOff>
+      <xdr:rowOff>1083419</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -720,7 +723,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1044272</xdr:colOff>
+      <xdr:colOff>1048082</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>1107627</xdr:rowOff>
     </xdr:to>
@@ -764,9 +767,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1388465</xdr:colOff>
+      <xdr:colOff>1392275</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>1006083</xdr:rowOff>
+      <xdr:rowOff>1009893</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -808,9 +811,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1427358</xdr:colOff>
+      <xdr:colOff>1431168</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>974725</xdr:rowOff>
+      <xdr:rowOff>970915</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -852,9 +855,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1165225</xdr:colOff>
+      <xdr:colOff>1161415</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>1008381</xdr:rowOff>
+      <xdr:rowOff>1012191</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -898,7 +901,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>1337309</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1618129</xdr:rowOff>
+      <xdr:rowOff>1621939</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -959,7 +962,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>2920</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>930405</xdr:rowOff>
+      <xdr:rowOff>934215</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1018,7 +1021,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1275901</xdr:colOff>
+      <xdr:colOff>1279711</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>1184462</xdr:rowOff>
     </xdr:to>
@@ -1135,9 +1138,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1083780</xdr:colOff>
+      <xdr:colOff>1087590</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>590549</xdr:rowOff>
+      <xdr:rowOff>594359</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1196,9 +1199,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1238793</xdr:colOff>
+      <xdr:colOff>1234983</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>968568</xdr:rowOff>
+      <xdr:rowOff>972378</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1240,7 +1243,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1392345</xdr:colOff>
+      <xdr:colOff>1388535</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>724397</xdr:rowOff>
     </xdr:to>
@@ -1284,9 +1287,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1241729</xdr:colOff>
+      <xdr:colOff>1237919</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>1088121</xdr:rowOff>
+      <xdr:rowOff>1084311</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1328,9 +1331,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>895796</xdr:colOff>
+      <xdr:colOff>891986</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>1121208</xdr:rowOff>
+      <xdr:rowOff>1125018</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1372,9 +1375,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1378175</xdr:colOff>
+      <xdr:colOff>1380080</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>973125</xdr:rowOff>
+      <xdr:rowOff>969315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1410,15 +1413,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>382415</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>631536</xdr:rowOff>
+      <xdr:colOff>254780</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1035396</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1208109</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>1345543</xdr:rowOff>
+      <xdr:colOff>1082379</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1755118</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1441,8 +1444,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8789263" y="8193558"/>
-          <a:ext cx="825694" cy="714007"/>
+          <a:off x="8893955" y="6407496"/>
+          <a:ext cx="831409" cy="719722"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1460,9 +1463,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1241481</xdr:colOff>
+      <xdr:colOff>1237671</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>999439</xdr:rowOff>
+      <xdr:rowOff>1001344</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1487,6 +1490,50 @@
         <a:xfrm>
           <a:off x="8592745" y="9589593"/>
           <a:ext cx="1030736" cy="934846"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>695326</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1259779</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1969771</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0114840E-7EF6-486A-92BD-70261B32D911}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8667750" y="8258176"/>
+          <a:ext cx="993079" cy="1276350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1821,25 +1868,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B20"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="D1" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="2" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="36.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="21.5546875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="9.109375" style="1"/>
+    <col min="12" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
@@ -1862,12 +1909,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
+    <row r="4" spans="2:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>12</v>
@@ -1883,10 +1930,10 @@
       </c>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="2:17" ht="156.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="20"/>
+    <row r="5" spans="2:17" ht="156.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="18"/>
       <c r="C5" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>16</v>
@@ -1902,10 +1949,10 @@
       </c>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="2:17" ht="156.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="20"/>
+    <row r="6" spans="2:17" ht="156.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="18"/>
       <c r="C6" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>21</v>
@@ -1921,10 +1968,10 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="2:17" ht="156.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="20"/>
+    <row r="7" spans="2:17" ht="156.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="18"/>
       <c r="C7" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>46</v>
@@ -1940,10 +1987,10 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="2:17" ht="156.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="20"/>
+    <row r="8" spans="2:17" ht="156.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="18"/>
       <c r="C8" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>46</v>
@@ -1955,34 +2002,34 @@
         <v>52</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="H8" s="14"/>
     </row>
-    <row r="9" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="20"/>
-      <c r="C9" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="19" t="s">
+    <row r="9" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="18"/>
+      <c r="C9" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="17" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>20</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
+    <row r="10" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="8" t="s">
         <v>38</v>
       </c>
@@ -1991,11 +2038,11 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
+    <row r="11" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
       <c r="F11" s="9" t="s">
         <v>39</v>
       </c>
@@ -2004,11 +2051,11 @@
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
+    <row r="12" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="9" t="s">
         <v>50</v>
       </c>
@@ -2017,15 +2064,15 @@
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="20"/>
-      <c r="C13" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="19" t="s">
+    <row r="13" spans="2:17" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="18"/>
+      <c r="C13" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="17" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="9" t="s">
@@ -2036,11 +2083,11 @@
       </c>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="2:17" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
+    <row r="14" spans="2:17" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="9" t="s">
         <v>28</v>
       </c>
@@ -2051,17 +2098,17 @@
       <c r="I14"/>
       <c r="Q14"/>
     </row>
-    <row r="15" spans="2:17" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="22" t="s">
+    <row r="15" spans="2:17" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="19" t="s">
+      <c r="C15" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="17" t="s">
         <v>22</v>
       </c>
       <c r="F15" s="8" t="s">
@@ -2072,11 +2119,11 @@
       </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="2:17" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
+    <row r="16" spans="2:17" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="8" t="s">
         <v>41</v>
       </c>
@@ -2085,11 +2132,11 @@
       </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="2:12" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
+    <row r="17" spans="2:12" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="8" t="s">
         <v>42</v>
       </c>
@@ -2098,12 +2145,12 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="2:12" ht="98.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="16" t="s">
-        <v>54</v>
+    <row r="18" spans="2:12" ht="98.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="21" t="s">
+        <v>53</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>34</v>
@@ -2120,15 +2167,15 @@
       <c r="H18" s="3"/>
       <c r="L18"/>
     </row>
-    <row r="19" spans="2:12" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
-      <c r="C19" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="19" t="s">
+    <row r="19" spans="2:12" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="22"/>
+      <c r="C19" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="17" t="s">
         <v>22</v>
       </c>
       <c r="F19" s="9" t="s">
@@ -2141,11 +2188,11 @@
       <c r="J19"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="18"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
+    <row r="20" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="23"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
       <c r="F20" s="9" t="s">
         <v>24</v>
       </c>
@@ -2155,46 +2202,46 @@
       <c r="H20" s="3"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="2:12" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="23"/>
+    <row r="21" spans="2:12" ht="82.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="16"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="2:12" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="23"/>
+    <row r="22" spans="2:12" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="16"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="2:12" s="12" customFormat="1" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="23"/>
+    <row r="23" spans="2:12" s="12" customFormat="1" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="16"/>
       <c r="K23" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B4:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="E15:E17"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="D9:D12"/>
     <mergeCell ref="E9:E12"/>
-    <mergeCell ref="B4:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="B18:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="35" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -2205,7 +2252,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2217,7 +2264,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>